<commit_message>
finished distribution-based inputation of negative one values, now onto cleaning rest of dfs
</commit_message>
<xml_diff>
--- a/SEC/data/StudentData/Spring_2023_Student_Feedback_Responses.xlsx
+++ b/SEC/data/StudentData/Spring_2023_Student_Feedback_Responses.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="247">
   <si>
     <t>major</t>
   </si>
@@ -80,9 +80,6 @@
   </si>
   <si>
     <t>add_info</t>
-  </si>
-  <si>
-    <t>add_comm</t>
   </si>
   <si>
     <t>Other</t>
@@ -261,9 +258,6 @@
     <t>Make the company list easier to see. It should be front page. I don’t know to what extent the career fair team has control over this, but Ocean Engineering is always at the bottom of alphabetical lists. Many sponsors don’t put OCEN as a major they are hiring, because they don’t know it exists, and they won’t find it without explicitly searching for it. This is to the detriment of the sponsor and the students.</t>
   </si>
   <si>
-    <t>Staff is good</t>
-  </si>
-  <si>
     <t>Aerospace Engineering</t>
   </si>
   <si>
@@ -307,9 +301,6 @@
   </si>
   <si>
     <t>That the career fair was split between two areas</t>
-  </si>
-  <si>
-    <t>N/A</t>
   </si>
   <si>
     <t>Chemical Engineering</t>
@@ -456,12 +447,6 @@
   </si>
   <si>
     <t>SEC Career Fair Website (https://careerfair.sec.tamu.edu/), Texas A&amp;M Career Center (https://careercenter.tamu.edu/), College of Engineering Weekly Emails, Other</t>
-  </si>
-  <si>
-    <t>Nothing comes to mind. Keep up the great work!</t>
-  </si>
-  <si>
-    <t>everything was really well put together and it was easy to get and find the information that I needed</t>
   </si>
   <si>
     <t>Updated and printed your resume, Looked at the list of companies attending, Researched companies</t>
@@ -559,9 +544,6 @@
     <t>bus stops at zach. provide a better transportation from Zach to Kyle Field</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>Updated and printed your resume, Looked at the list of companies attending, Researched companies, Applied to companies attending online</t>
   </si>
   <si>
@@ -713,9 +695,6 @@
     <t>Please try to invite more companies to our Career Fair.</t>
   </si>
   <si>
-    <t>Nothing to add.</t>
-  </si>
-  <si>
     <t>Four</t>
   </si>
   <si>
@@ -729,9 +708,6 @@
   </si>
   <si>
     <t>I didn't know about the two different areas or how selecting a company to go in a specific area worked so further information on that would be helpful.</t>
-  </si>
-  <si>
-    <t>I don't have any other suggestions but the people helping at the career fair were very nice.</t>
   </si>
   <si>
     <t>Marathon was the best!</t>
@@ -799,6 +775,9 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>Nothing comes to mind. Keep up the great work! Everything was really well put together and it was easy to get and find the information that I needed</t>
   </si>
 </sst>
 </file>
@@ -1143,20 +1122,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X54"/>
+  <dimension ref="A1:W54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AB9" sqref="AB9"/>
+    <sheetView tabSelected="1" topLeftCell="W1" zoomScale="77" workbookViewId="0">
+      <selection activeCell="W26" sqref="W26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="173.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="255.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="51.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="71.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="253.21875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="255.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1224,84 +1208,81 @@
       <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
         <v>24</v>
-      </c>
-      <c r="D2" t="s">
-        <v>25</v>
       </c>
       <c r="E2">
         <v>6</v>
       </c>
       <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
+      <c r="H2">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
         <v>26</v>
       </c>
-      <c r="G2">
-        <v>4</v>
-      </c>
-      <c r="H2">
-        <v>4</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>27</v>
       </c>
-      <c r="J2" t="s">
-        <v>28</v>
-      </c>
       <c r="K2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" t="s">
+        <v>28</v>
+      </c>
+      <c r="R2">
+        <v>3</v>
+      </c>
+      <c r="S2" t="s">
         <v>29</v>
       </c>
-      <c r="L2" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" t="s">
-        <v>29</v>
-      </c>
-      <c r="R2">
-        <v>3</v>
-      </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>30</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>31</v>
-      </c>
-      <c r="U2" t="s">
-        <v>32</v>
       </c>
       <c r="V2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
         <v>33</v>
-      </c>
-      <c r="C3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" t="s">
-        <v>34</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G3">
         <v>4</v>
@@ -1310,51 +1291,51 @@
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3" t="s">
+        <v>28</v>
+      </c>
+      <c r="R3">
+        <v>3</v>
+      </c>
+      <c r="S3" t="s">
         <v>36</v>
       </c>
-      <c r="K3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L3" t="s">
-        <v>29</v>
-      </c>
-      <c r="O3" t="s">
-        <v>29</v>
-      </c>
-      <c r="R3">
-        <v>3</v>
-      </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
+        <v>30</v>
+      </c>
+      <c r="V3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>37</v>
       </c>
-      <c r="T3" t="s">
-        <v>31</v>
-      </c>
-      <c r="V3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
         <v>38</v>
       </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="E4">
-        <v>5</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="G4">
         <v>5</v>
@@ -1363,51 +1344,51 @@
         <v>13</v>
       </c>
       <c r="I4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R4">
+        <v>5</v>
+      </c>
+      <c r="S4" t="s">
         <v>41</v>
       </c>
-      <c r="K4" t="s">
-        <v>29</v>
-      </c>
-      <c r="L4" t="s">
-        <v>29</v>
-      </c>
-      <c r="O4" t="s">
-        <v>29</v>
-      </c>
-      <c r="R4">
-        <v>5</v>
-      </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>42</v>
       </c>
-      <c r="T4" t="s">
+      <c r="V4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>43</v>
       </c>
-      <c r="V4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
         <v>44</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>45</v>
       </c>
       <c r="E5">
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G5">
         <v>2</v>
@@ -1416,104 +1397,104 @@
         <v>10</v>
       </c>
       <c r="I5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R5">
         <v>1</v>
       </c>
       <c r="S5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="V5">
         <v>2</v>
       </c>
       <c r="W5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="s">
-        <v>50</v>
       </c>
       <c r="E6">
         <v>10</v>
       </c>
       <c r="F6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G6">
-        <v>3</v>
-      </c>
-      <c r="H6">
-        <v>4</v>
-      </c>
-      <c r="I6" t="s">
-        <v>27</v>
-      </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" t="s">
+        <v>28</v>
+      </c>
+      <c r="O6" t="s">
+        <v>28</v>
+      </c>
+      <c r="R6">
+        <v>3</v>
+      </c>
+      <c r="S6" t="s">
         <v>52</v>
       </c>
-      <c r="K6" t="s">
-        <v>29</v>
-      </c>
-      <c r="L6" t="s">
-        <v>29</v>
-      </c>
-      <c r="O6" t="s">
-        <v>29</v>
-      </c>
-      <c r="R6">
-        <v>3</v>
-      </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>53</v>
       </c>
-      <c r="T6" t="s">
-        <v>54</v>
-      </c>
       <c r="V6">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
         <v>55</v>
       </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
         <v>56</v>
-      </c>
-      <c r="E7">
-        <v>5</v>
-      </c>
-      <c r="F7" t="s">
-        <v>57</v>
       </c>
       <c r="G7">
         <v>5</v>
@@ -1522,110 +1503,110 @@
         <v>6</v>
       </c>
       <c r="I7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J7" t="s">
+        <v>57</v>
+      </c>
+      <c r="K7" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7" t="s">
+        <v>28</v>
+      </c>
+      <c r="O7" t="s">
+        <v>28</v>
+      </c>
+      <c r="R7">
+        <v>5</v>
+      </c>
+      <c r="S7" t="s">
         <v>58</v>
       </c>
-      <c r="K7" t="s">
-        <v>29</v>
-      </c>
-      <c r="L7" t="s">
-        <v>29</v>
-      </c>
-      <c r="O7" t="s">
-        <v>29</v>
-      </c>
-      <c r="R7">
-        <v>5</v>
-      </c>
-      <c r="S7" t="s">
-        <v>59</v>
-      </c>
       <c r="T7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V7">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
         <v>60</v>
       </c>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
         <v>61</v>
       </c>
-      <c r="E8">
-        <v>3</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="G8">
+        <v>4</v>
+      </c>
+      <c r="H8">
+        <v>4</v>
+      </c>
+      <c r="I8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" t="s">
         <v>62</v>
       </c>
-      <c r="G8">
-        <v>4</v>
-      </c>
-      <c r="H8">
-        <v>4</v>
-      </c>
-      <c r="I8" t="s">
-        <v>27</v>
-      </c>
-      <c r="J8" t="s">
-        <v>63</v>
-      </c>
       <c r="K8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R8">
         <v>2</v>
       </c>
       <c r="S8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U8" t="s">
+        <v>63</v>
+      </c>
+      <c r="V8">
+        <v>4</v>
+      </c>
+      <c r="W8" t="s">
         <v>64</v>
       </c>
-      <c r="V8">
-        <v>4</v>
-      </c>
-      <c r="W8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
         <v>38</v>
-      </c>
-      <c r="C9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" t="s">
-        <v>39</v>
       </c>
       <c r="E9">
         <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G9">
         <v>4</v>
@@ -1634,51 +1615,51 @@
         <v>15</v>
       </c>
       <c r="I9" t="s">
+        <v>66</v>
+      </c>
+      <c r="J9" t="s">
         <v>67</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L9" t="s">
+        <v>28</v>
+      </c>
+      <c r="O9" t="s">
+        <v>28</v>
+      </c>
+      <c r="R9">
+        <v>3</v>
+      </c>
+      <c r="S9" t="s">
         <v>68</v>
       </c>
-      <c r="K9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L9" t="s">
-        <v>29</v>
-      </c>
-      <c r="O9" t="s">
-        <v>29</v>
-      </c>
-      <c r="R9">
-        <v>3</v>
-      </c>
-      <c r="S9" t="s">
-        <v>69</v>
-      </c>
       <c r="T9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="V9">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G10">
         <v>3</v>
@@ -1687,51 +1668,51 @@
         <v>8</v>
       </c>
       <c r="I10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R10">
         <v>2</v>
       </c>
       <c r="S10" t="s">
+        <v>72</v>
+      </c>
+      <c r="T10" t="s">
+        <v>42</v>
+      </c>
+      <c r="U10" t="s">
         <v>73</v>
-      </c>
-      <c r="T10" t="s">
-        <v>43</v>
-      </c>
-      <c r="U10" t="s">
-        <v>74</v>
       </c>
       <c r="V10">
         <v>2</v>
       </c>
       <c r="W10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s">
         <v>76</v>
-      </c>
-      <c r="C11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" t="s">
-        <v>77</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -1746,60 +1727,57 @@
         <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R11">
         <v>2</v>
       </c>
       <c r="S11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="U11" t="s">
+        <v>78</v>
+      </c>
+      <c r="V11">
+        <v>3</v>
+      </c>
+      <c r="W11" t="s">
         <v>79</v>
       </c>
-      <c r="V11">
-        <v>3</v>
-      </c>
-      <c r="W11" t="s">
-        <v>80</v>
-      </c>
-      <c r="X11" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>81</v>
+      </c>
+      <c r="E12" t="s">
         <v>82</v>
       </c>
-      <c r="C12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="F12" t="s">
         <v>83</v>
-      </c>
-      <c r="E12" t="s">
-        <v>84</v>
-      </c>
-      <c r="F12" t="s">
-        <v>85</v>
       </c>
       <c r="G12">
         <v>5</v>
@@ -1808,107 +1786,107 @@
         <v>7</v>
       </c>
       <c r="I12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J12" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R12">
         <v>5</v>
       </c>
       <c r="S12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="V12">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E13">
         <v>2</v>
       </c>
       <c r="F13" t="s">
+        <v>86</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+      <c r="H13">
+        <v>3</v>
+      </c>
+      <c r="I13" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" t="s">
+        <v>87</v>
+      </c>
+      <c r="K13" t="s">
+        <v>28</v>
+      </c>
+      <c r="L13" t="s">
+        <v>28</v>
+      </c>
+      <c r="O13" t="s">
+        <v>28</v>
+      </c>
+      <c r="R13">
+        <v>5</v>
+      </c>
+      <c r="S13" t="s">
         <v>88</v>
       </c>
-      <c r="G13">
-        <v>4</v>
-      </c>
-      <c r="H13">
-        <v>3</v>
-      </c>
-      <c r="I13" t="s">
-        <v>27</v>
-      </c>
-      <c r="J13" t="s">
+      <c r="T13" t="s">
+        <v>42</v>
+      </c>
+      <c r="V13">
+        <v>5</v>
+      </c>
+      <c r="W13" t="s">
         <v>89</v>
       </c>
-      <c r="K13" t="s">
-        <v>29</v>
-      </c>
-      <c r="L13" t="s">
-        <v>29</v>
-      </c>
-      <c r="O13" t="s">
-        <v>29</v>
-      </c>
-      <c r="R13">
-        <v>5</v>
-      </c>
-      <c r="S13" t="s">
-        <v>90</v>
-      </c>
-      <c r="T13" t="s">
-        <v>43</v>
-      </c>
-      <c r="V13">
-        <v>5</v>
-      </c>
-      <c r="X13" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E14">
         <v>3</v>
       </c>
       <c r="F14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G14">
         <v>5</v>
@@ -1917,60 +1895,57 @@
         <v>8</v>
       </c>
       <c r="I14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J14" t="s">
+        <v>91</v>
+      </c>
+      <c r="K14" t="s">
+        <v>28</v>
+      </c>
+      <c r="L14" t="s">
+        <v>28</v>
+      </c>
+      <c r="O14" t="s">
+        <v>28</v>
+      </c>
+      <c r="R14">
+        <v>4</v>
+      </c>
+      <c r="S14" t="s">
+        <v>92</v>
+      </c>
+      <c r="T14" t="s">
+        <v>30</v>
+      </c>
+      <c r="U14" t="s">
         <v>93</v>
       </c>
-      <c r="K14" t="s">
-        <v>29</v>
-      </c>
-      <c r="L14" t="s">
-        <v>29</v>
-      </c>
-      <c r="O14" t="s">
-        <v>29</v>
-      </c>
-      <c r="R14">
-        <v>4</v>
-      </c>
-      <c r="S14" t="s">
+      <c r="V14">
+        <v>5</v>
+      </c>
+      <c r="W14" t="s">
         <v>94</v>
       </c>
-      <c r="T14" t="s">
-        <v>31</v>
-      </c>
-      <c r="U14" t="s">
-        <v>95</v>
-      </c>
-      <c r="V14">
-        <v>5</v>
-      </c>
-      <c r="W14" t="s">
-        <v>96</v>
-      </c>
-      <c r="X14" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E15" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F15" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="G15">
         <v>5</v>
@@ -1979,54 +1954,54 @@
         <v>20</v>
       </c>
       <c r="I15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J15" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R15">
         <v>4</v>
       </c>
       <c r="S15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="T15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U15" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="V15">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D16" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E16">
         <v>5</v>
       </c>
       <c r="F16" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G16">
         <v>4</v>
@@ -2035,63 +2010,63 @@
         <v>15</v>
       </c>
       <c r="I16" t="s">
+        <v>101</v>
+      </c>
+      <c r="J16" t="s">
+        <v>102</v>
+      </c>
+      <c r="K16" t="s">
+        <v>23</v>
+      </c>
+      <c r="L16" t="s">
+        <v>28</v>
+      </c>
+      <c r="O16" t="s">
+        <v>23</v>
+      </c>
+      <c r="P16">
+        <v>4</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>103</v>
+      </c>
+      <c r="R16">
+        <v>5</v>
+      </c>
+      <c r="S16" t="s">
         <v>104</v>
       </c>
-      <c r="J16" t="s">
+      <c r="T16" t="s">
+        <v>30</v>
+      </c>
+      <c r="U16" t="s">
         <v>105</v>
       </c>
-      <c r="K16" t="s">
-        <v>24</v>
-      </c>
-      <c r="L16" t="s">
-        <v>29</v>
-      </c>
-      <c r="O16" t="s">
-        <v>24</v>
-      </c>
-      <c r="P16">
-        <v>4</v>
-      </c>
-      <c r="Q16" t="s">
+      <c r="V16">
+        <v>4</v>
+      </c>
+      <c r="W16" t="s">
         <v>106</v>
       </c>
-      <c r="R16">
-        <v>5</v>
-      </c>
-      <c r="S16" t="s">
-        <v>107</v>
-      </c>
-      <c r="T16" t="s">
-        <v>31</v>
-      </c>
-      <c r="U16" t="s">
-        <v>108</v>
-      </c>
-      <c r="V16">
-        <v>4</v>
-      </c>
-      <c r="W16" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" t="s">
         <v>24</v>
       </c>
-      <c r="D17" t="s">
-        <v>25</v>
-      </c>
       <c r="E17" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F17" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G17">
         <v>5</v>
@@ -2100,45 +2075,45 @@
         <v>12</v>
       </c>
       <c r="I17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J17" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="K17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R17">
         <v>4</v>
       </c>
       <c r="S17" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="T17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V17">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D18" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E18">
         <v>4</v>
@@ -2153,101 +2128,101 @@
         <v>8</v>
       </c>
       <c r="I18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J18" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="K18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R18">
         <v>5</v>
       </c>
       <c r="S18" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="T18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V18">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D19" t="s">
+        <v>114</v>
+      </c>
+      <c r="E19" t="s">
+        <v>115</v>
+      </c>
+      <c r="F19" t="s">
+        <v>116</v>
+      </c>
+      <c r="G19">
+        <v>4</v>
+      </c>
+      <c r="H19">
+        <v>4</v>
+      </c>
+      <c r="I19" t="s">
+        <v>66</v>
+      </c>
+      <c r="J19" t="s">
         <v>117</v>
       </c>
-      <c r="E19" t="s">
-        <v>118</v>
-      </c>
-      <c r="F19" t="s">
-        <v>119</v>
-      </c>
-      <c r="G19">
-        <v>4</v>
-      </c>
-      <c r="H19">
-        <v>4</v>
-      </c>
-      <c r="I19" t="s">
-        <v>67</v>
-      </c>
-      <c r="J19" t="s">
-        <v>120</v>
-      </c>
       <c r="K19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R19">
         <v>4</v>
       </c>
       <c r="S19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V19">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E20">
         <v>15</v>
       </c>
       <c r="F20" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G20">
         <v>4</v>
@@ -2256,54 +2231,54 @@
         <v>8</v>
       </c>
       <c r="I20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J20" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="K20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R20">
         <v>3</v>
       </c>
       <c r="S20" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="T20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V20">
         <v>4</v>
       </c>
       <c r="W20" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="21" spans="1:24" ht="43.2" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E21">
         <v>7</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G21">
         <v>5</v>
@@ -2312,116 +2287,113 @@
         <v>6</v>
       </c>
       <c r="I21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J21" t="s">
+        <v>123</v>
+      </c>
+      <c r="K21" t="s">
+        <v>28</v>
+      </c>
+      <c r="L21" t="s">
+        <v>28</v>
+      </c>
+      <c r="O21" t="s">
+        <v>28</v>
+      </c>
+      <c r="R21">
+        <v>4</v>
+      </c>
+      <c r="S21" t="s">
+        <v>124</v>
+      </c>
+      <c r="T21" t="s">
+        <v>125</v>
+      </c>
+      <c r="U21" t="s">
         <v>126</v>
       </c>
-      <c r="K21" t="s">
-        <v>29</v>
-      </c>
-      <c r="L21" t="s">
-        <v>29</v>
-      </c>
-      <c r="O21" t="s">
-        <v>29</v>
-      </c>
-      <c r="R21">
-        <v>4</v>
-      </c>
-      <c r="S21" t="s">
-        <v>127</v>
-      </c>
-      <c r="T21" t="s">
-        <v>128</v>
-      </c>
-      <c r="U21" t="s">
-        <v>129</v>
-      </c>
       <c r="V21">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D22" t="s">
+        <v>127</v>
+      </c>
+      <c r="E22">
+        <v>4</v>
+      </c>
+      <c r="F22" t="s">
+        <v>128</v>
+      </c>
+      <c r="G22">
+        <v>4</v>
+      </c>
+      <c r="H22">
+        <v>4</v>
+      </c>
+      <c r="I22" t="s">
+        <v>66</v>
+      </c>
+      <c r="J22" t="s">
+        <v>129</v>
+      </c>
+      <c r="K22" t="s">
+        <v>28</v>
+      </c>
+      <c r="L22" t="s">
+        <v>28</v>
+      </c>
+      <c r="O22" t="s">
+        <v>28</v>
+      </c>
+      <c r="R22">
+        <v>4</v>
+      </c>
+      <c r="S22" t="s">
         <v>130</v>
       </c>
-      <c r="E22">
-        <v>4</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="T22" t="s">
+        <v>30</v>
+      </c>
+      <c r="U22" t="s">
+        <v>63</v>
+      </c>
+      <c r="V22">
+        <v>4</v>
+      </c>
+      <c r="W22" t="s">
         <v>131</v>
       </c>
-      <c r="G22">
-        <v>4</v>
-      </c>
-      <c r="H22">
-        <v>4</v>
-      </c>
-      <c r="I22" t="s">
-        <v>67</v>
-      </c>
-      <c r="J22" t="s">
-        <v>132</v>
-      </c>
-      <c r="K22" t="s">
-        <v>29</v>
-      </c>
-      <c r="L22" t="s">
-        <v>29</v>
-      </c>
-      <c r="O22" t="s">
-        <v>29</v>
-      </c>
-      <c r="R22">
-        <v>4</v>
-      </c>
-      <c r="S22" t="s">
-        <v>133</v>
-      </c>
-      <c r="T22" t="s">
-        <v>31</v>
-      </c>
-      <c r="U22" t="s">
-        <v>64</v>
-      </c>
-      <c r="V22">
-        <v>4</v>
-      </c>
-      <c r="W22" t="s">
-        <v>134</v>
-      </c>
-      <c r="X22" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D23" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E23">
         <v>2</v>
       </c>
       <c r="F23" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="G23">
         <v>5</v>
@@ -2430,51 +2402,51 @@
         <v>3</v>
       </c>
       <c r="I23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J23" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="K23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R23">
         <v>4</v>
       </c>
       <c r="S23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V23">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E24">
         <v>18</v>
       </c>
       <c r="F24" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="G24">
         <v>4</v>
@@ -2483,110 +2455,107 @@
         <v>25</v>
       </c>
       <c r="I24" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="J24" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="K24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R24">
         <v>4</v>
       </c>
       <c r="S24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="T24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V24">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D25" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E25">
         <v>8</v>
       </c>
       <c r="F25" t="s">
+        <v>139</v>
+      </c>
+      <c r="G25">
+        <v>5</v>
+      </c>
+      <c r="H25" t="s">
+        <v>140</v>
+      </c>
+      <c r="I25" t="s">
+        <v>66</v>
+      </c>
+      <c r="J25" t="s">
+        <v>141</v>
+      </c>
+      <c r="K25" t="s">
+        <v>28</v>
+      </c>
+      <c r="L25" t="s">
+        <v>28</v>
+      </c>
+      <c r="O25" t="s">
+        <v>28</v>
+      </c>
+      <c r="R25">
+        <v>4</v>
+      </c>
+      <c r="S25" t="s">
         <v>142</v>
       </c>
-      <c r="G25">
-        <v>5</v>
-      </c>
-      <c r="H25" t="s">
-        <v>143</v>
-      </c>
-      <c r="I25" t="s">
-        <v>67</v>
-      </c>
-      <c r="J25" t="s">
-        <v>144</v>
-      </c>
-      <c r="K25" t="s">
-        <v>29</v>
-      </c>
-      <c r="L25" t="s">
-        <v>29</v>
-      </c>
-      <c r="O25" t="s">
-        <v>29</v>
-      </c>
-      <c r="R25">
-        <v>4</v>
-      </c>
-      <c r="S25" t="s">
-        <v>145</v>
-      </c>
       <c r="T25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V25">
         <v>5</v>
       </c>
       <c r="W25" t="s">
-        <v>146</v>
-      </c>
-      <c r="X25" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D26" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="E26">
         <v>4</v>
       </c>
       <c r="F26" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="G26">
         <v>5</v>
@@ -2595,57 +2564,57 @@
         <v>6</v>
       </c>
       <c r="I26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J26" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="K26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R26">
         <v>5</v>
       </c>
       <c r="S26" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="T26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="U26" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="V26">
         <v>5</v>
       </c>
       <c r="W26" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="27" spans="1:24" ht="172.8" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E27">
         <v>8</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="G27">
         <v>5</v>
@@ -2654,54 +2623,54 @@
         <v>8</v>
       </c>
       <c r="I27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J27" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="K27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R27">
         <v>3</v>
       </c>
       <c r="S27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="T27" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V27">
         <v>3</v>
       </c>
       <c r="W27" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D28" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E28">
         <v>5</v>
       </c>
       <c r="F28" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G28">
         <v>4</v>
@@ -2710,54 +2679,54 @@
         <v>15</v>
       </c>
       <c r="I28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J28" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="K28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R28">
         <v>5</v>
       </c>
       <c r="S28" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="T28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V28">
         <v>4</v>
       </c>
       <c r="W28" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D29" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="E29">
         <v>6</v>
       </c>
       <c r="F29" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="G29">
         <v>4</v>
@@ -2766,57 +2735,54 @@
         <v>12</v>
       </c>
       <c r="I29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J29" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="K29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R29">
         <v>5</v>
       </c>
       <c r="S29" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="T29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V29">
         <v>5</v>
       </c>
       <c r="W29" t="s">
-        <v>164</v>
-      </c>
-      <c r="X29" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="C30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E30">
         <v>5</v>
       </c>
       <c r="F30" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="G30">
         <v>4</v>
@@ -2825,51 +2791,51 @@
         <v>7</v>
       </c>
       <c r="I30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J30" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="K30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R30">
         <v>5</v>
       </c>
       <c r="S30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="T30" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V30">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E31">
         <v>2</v>
       </c>
       <c r="F31" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="G31">
         <v>4</v>
@@ -2878,7 +2844,7 @@
         <v>10</v>
       </c>
       <c r="I31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J31" t="e">
         <f>- notify students when headshots close
@@ -2886,42 +2852,42 @@
         <v>#NAME?</v>
       </c>
       <c r="K31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R31">
         <v>3</v>
       </c>
       <c r="S31" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="T31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V31">
         <v>4</v>
       </c>
       <c r="W31" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D32" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -2933,48 +2899,48 @@
         <v>4</v>
       </c>
       <c r="I32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J32" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="K32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R32">
         <v>3</v>
       </c>
       <c r="S32" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V32">
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D33" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="E33">
         <v>3</v>
       </c>
       <c r="F33" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="G33">
         <v>5</v>
@@ -2983,60 +2949,57 @@
         <v>4</v>
       </c>
       <c r="I33" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J33" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="K33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R33">
         <v>4</v>
       </c>
       <c r="S33" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="T33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U33" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="V33">
         <v>4</v>
       </c>
       <c r="W33" t="s">
-        <v>177</v>
-      </c>
-      <c r="X33" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="34" spans="1:24" ht="230.4" x14ac:dyDescent="0.3">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C34" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D34" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E34">
         <v>7</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="G34">
         <v>3</v>
@@ -3045,22 +3008,22 @@
         <v>30</v>
       </c>
       <c r="I34" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="K34" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L34" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M34">
         <v>4</v>
       </c>
       <c r="O34" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P34">
         <v>4</v>
@@ -3069,27 +3032,27 @@
         <v>5</v>
       </c>
       <c r="S34" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="T34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V34">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C35" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E35">
         <v>6</v>
@@ -3101,51 +3064,51 @@
         <v>9</v>
       </c>
       <c r="I35" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J35" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="K35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R35">
         <v>2</v>
       </c>
       <c r="S35" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="T35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V35">
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D36" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="E36">
         <v>12</v>
       </c>
       <c r="F36" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="G36">
         <v>3</v>
@@ -3154,48 +3117,48 @@
         <v>20</v>
       </c>
       <c r="I36" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J36" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="K36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R36">
         <v>2</v>
       </c>
       <c r="S36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V36">
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C37" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D37" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E37">
         <v>10</v>
       </c>
       <c r="F37" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="G37">
         <v>5</v>
@@ -3204,104 +3167,104 @@
         <v>8</v>
       </c>
       <c r="I37" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J37" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="K37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R37">
         <v>4</v>
       </c>
       <c r="S37" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="T37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="V37">
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C38" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E38">
         <v>3</v>
       </c>
       <c r="F38" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="G38">
         <v>3</v>
       </c>
       <c r="H38" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="I38" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J38" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="K38" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L38" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O38" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R38">
         <v>5</v>
       </c>
       <c r="S38" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="T38" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V38">
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C39" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E39">
         <v>6</v>
       </c>
       <c r="F39" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="G39">
         <v>5</v>
@@ -3310,57 +3273,57 @@
         <v>15</v>
       </c>
       <c r="I39" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J39" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="K39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R39">
         <v>5</v>
       </c>
       <c r="S39" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="T39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="U39" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="V39">
         <v>5</v>
       </c>
       <c r="W39" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="40" spans="1:24" ht="409.6" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C40" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E40">
         <v>2</v>
       </c>
       <c r="F40" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="G40">
         <v>1</v>
@@ -3369,51 +3332,51 @@
         <v>3</v>
       </c>
       <c r="I40" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="K40" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L40" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O40" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R40">
         <v>1</v>
       </c>
       <c r="S40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="T40" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V40">
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:24" ht="72" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:23" ht="72" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C41" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D41" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E41">
         <v>3</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="G41">
         <v>4</v>
@@ -3422,48 +3385,48 @@
         <v>5</v>
       </c>
       <c r="I41" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J41" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="K41" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L41" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O41" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R41">
         <v>4</v>
       </c>
       <c r="S41" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="V41">
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E42">
         <v>3</v>
       </c>
       <c r="F42" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="G42">
         <v>3</v>
@@ -3472,45 +3435,45 @@
         <v>5</v>
       </c>
       <c r="I42" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J42" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="K42" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L42" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O42" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R42">
         <v>3</v>
       </c>
       <c r="S42" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="T42" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V42">
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C43" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D43" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="E43">
         <v>2</v>
@@ -3525,57 +3488,57 @@
         <v>2</v>
       </c>
       <c r="I43" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J43" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="K43" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L43" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O43" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R43">
         <v>4</v>
       </c>
       <c r="S43" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="T43" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="U43" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="V43">
         <v>4</v>
       </c>
       <c r="W43" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="44" spans="1:24" ht="100.8" x14ac:dyDescent="0.3">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C44" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D44" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E44">
         <v>9</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="G44">
         <v>5</v>
@@ -3584,22 +3547,22 @@
         <v>10</v>
       </c>
       <c r="I44" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J44" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="K44" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L44" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M44">
         <v>5</v>
       </c>
       <c r="O44" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P44">
         <v>5</v>
@@ -3608,36 +3571,36 @@
         <v>4</v>
       </c>
       <c r="S44" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="T44" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V44">
         <v>5</v>
       </c>
-      <c r="X44" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="W44" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C45" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D45" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E45">
         <v>2</v>
       </c>
       <c r="F45" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="G45">
         <v>3</v>
@@ -3646,128 +3609,125 @@
         <v>15</v>
       </c>
       <c r="I45" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J45" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="K45" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L45" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O45" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R45">
         <v>1</v>
       </c>
       <c r="S45" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="T45" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U45" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="V45">
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C46" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D46" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E46">
         <v>3</v>
       </c>
       <c r="F46" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="G46">
         <v>3</v>
       </c>
       <c r="H46" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="I46" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="J46" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="K46" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L46" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M46">
         <v>1</v>
       </c>
       <c r="N46" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="O46" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P46">
         <v>5</v>
       </c>
       <c r="Q46" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="R46">
         <v>4</v>
       </c>
       <c r="S46" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="T46" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="U46" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="V46">
         <v>5</v>
       </c>
       <c r="W46" t="s">
-        <v>224</v>
-      </c>
-      <c r="X46" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C47" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D47" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E47" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="F47" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="G47">
         <v>4</v>
@@ -3776,60 +3736,57 @@
         <v>20</v>
       </c>
       <c r="I47" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J47" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="K47" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L47" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O47" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R47">
         <v>3</v>
       </c>
       <c r="S47" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="U47" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="V47">
         <v>3</v>
       </c>
       <c r="W47" t="s">
-        <v>230</v>
-      </c>
-      <c r="X47" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C48" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D48" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E48">
         <v>10</v>
       </c>
       <c r="F48" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="G48">
         <v>5</v>
@@ -3838,28 +3795,28 @@
         <v>15</v>
       </c>
       <c r="I48" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J48" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="K48" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L48" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O48" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R48">
         <v>5</v>
       </c>
       <c r="S48" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="T48" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V48">
         <v>5</v>
@@ -3870,19 +3827,19 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C49" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D49" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E49">
         <v>4</v>
       </c>
       <c r="F49" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="G49">
         <v>4</v>
@@ -3891,34 +3848,34 @@
         <v>6</v>
       </c>
       <c r="I49" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J49" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="K49" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L49" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O49" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R49">
         <v>4</v>
       </c>
       <c r="S49" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="T49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="V49">
         <v>4</v>
       </c>
       <c r="W49" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.3">
@@ -3926,19 +3883,19 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C50" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D50" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="E50">
         <v>10</v>
       </c>
       <c r="F50" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="G50">
         <v>4</v>
@@ -3947,37 +3904,37 @@
         <v>7</v>
       </c>
       <c r="I50" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J50" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="K50" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L50" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O50" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R50">
         <v>3</v>
       </c>
       <c r="S50" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="T50" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U50" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="V50">
         <v>3</v>
       </c>
       <c r="W50" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.3">
@@ -3985,19 +3942,19 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C51" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D51" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E51">
         <v>3</v>
       </c>
       <c r="F51" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="G51">
         <v>4</v>
@@ -4006,28 +3963,28 @@
         <v>6</v>
       </c>
       <c r="I51" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J51" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="K51" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L51" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O51" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R51">
         <v>3</v>
       </c>
       <c r="S51" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="T51" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V51">
         <v>2</v>
@@ -4038,19 +3995,19 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="C52" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D52" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E52">
         <v>3</v>
       </c>
       <c r="F52" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="G52">
         <v>4</v>
@@ -4059,28 +4016,28 @@
         <v>15</v>
       </c>
       <c r="I52" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J52" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="K52" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L52" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O52" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R52">
         <v>5</v>
       </c>
       <c r="S52" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="T52" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V52">
         <v>4</v>
@@ -4091,19 +4048,19 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C53" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D53" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="E53">
         <v>3</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="G53">
         <v>2</v>
@@ -4112,34 +4069,34 @@
         <v>6</v>
       </c>
       <c r="I53" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J53" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="K53" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L53" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O53" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R53">
         <v>3</v>
       </c>
       <c r="S53" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="T53" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V53">
         <v>3</v>
       </c>
       <c r="W53" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.3">
@@ -4147,19 +4104,19 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C54" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D54" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E54">
         <v>3</v>
       </c>
       <c r="F54" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="G54">
         <v>5</v>
@@ -4168,25 +4125,25 @@
         <v>8</v>
       </c>
       <c r="I54" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J54" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="K54" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L54" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O54" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="R54">
         <v>5</v>
       </c>
       <c r="S54" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="V54">
         <v>5</v>

</xml_diff>